<commit_message>
Formatação de hora e ingestão de dados manuais.
</commit_message>
<xml_diff>
--- a/data_bases/restaurants.xlsx
+++ b/data_bases/restaurants.xlsx
@@ -1332,7 +1332,11 @@
           <t>100</t>
         </is>
       </c>
-      <c r="G17" t="inlineStr"/>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>Álvaro Camargos</t>
+        </is>
+      </c>
       <c r="H17" t="inlineStr">
         <is>
           <t>BELO HORIZONTE</t>
@@ -6404,7 +6408,7 @@
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>ao creme, acompanhado de mandioca na manteiga de garrafa com queijo gratinado e bacon crocante.</t>
+          <t>Contrafilé flambado na cachaça ao creme, acompanhado de mandioca na manteiga de garrafa com queijo gratinado e bacon crocante.</t>
         </is>
       </c>
       <c r="E111" t="inlineStr">
@@ -7112,11 +7116,31 @@
           <t>Asinhas de frango com provolone com tempero.</t>
         </is>
       </c>
-      <c r="E124" t="inlineStr"/>
-      <c r="F124" t="inlineStr"/>
-      <c r="G124" t="inlineStr"/>
-      <c r="H124" t="inlineStr"/>
-      <c r="I124" t="inlineStr"/>
+      <c r="E124" t="inlineStr">
+        <is>
+          <t>Av Altamiro avelino Soares</t>
+        </is>
+      </c>
+      <c r="F124" t="inlineStr">
+        <is>
+          <t>920</t>
+        </is>
+      </c>
+      <c r="G124" t="inlineStr">
+        <is>
+          <t>Castelo</t>
+        </is>
+      </c>
+      <c r="H124" t="inlineStr">
+        <is>
+          <t>Belo Horizonte</t>
+        </is>
+      </c>
+      <c r="I124" t="inlineStr">
+        <is>
+          <t>MG</t>
+        </is>
+      </c>
       <c r="J124" t="inlineStr"/>
       <c r="K124" t="inlineStr">
         <is>

</xml_diff>